<commit_message>
Changes in excel files
</commit_message>
<xml_diff>
--- a/raw_files/basal_soil_respiration.xlsx
+++ b/raw_files/basal_soil_respiration.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raquel.correa\Desktop\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignacio.romero\ownCloud - Romero Ignacio@owncloud.fibl.org\exchange_iro_nbo_vgf\iro\banana_microbiome\raw_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7F866-D44D-4BBC-BF14-900A5CCBD2EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B0A8EA-AED0-4DB2-A638-496176F53366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{FD341CF6-027E-43AF-A64C-D1822CDDEC5D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{FD341CF6-027E-43AF-A64C-D1822CDDEC5D}"/>
   </bookViews>
   <sheets>
     <sheet name="basal" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -442,17 +441,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7303995-6BBF-4F5C-9F58-E49506BC2B82}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,7 +462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -474,7 +473,7 @@
         <v>16.988825128360013</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -485,7 +484,7 @@
         <v>7.5452716297786724</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -496,7 +495,7 @@
         <v>11.534518113465483</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -507,7 +506,7 @@
         <v>14.539218610199821</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -518,7 +517,7 @@
         <v>15.373699148533587</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -529,7 +528,7 @@
         <v>11.957908163265307</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -540,7 +539,7 @@
         <v>22.976459206707517</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -551,7 +550,7 @@
         <v>21.239773442416613</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -562,7 +561,7 @@
         <v>24.006064690026957</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -573,7 +572,7 @@
         <v>22.518963337547408</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -584,7 +583,7 @@
         <v>27.173913043478262</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -595,7 +594,7 @@
         <v>22.635814889336014</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -606,7 +605,7 @@
         <v>20.917260613572978</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -617,7 +616,7 @@
         <v>23.345347313237223</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -628,7 +627,7 @@
         <v>24.177129284017642</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -639,7 +638,7 @@
         <v>27.439024390243901</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -650,7 +649,7 @@
         <v>19.614253023864006</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -661,7 +660,7 @@
         <v>17.482517482517483</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -672,7 +671,7 @@
         <v>13.505402160864346</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -683,7 +682,7 @@
         <v>11.545566502463055</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -694,7 +693,7 @@
         <v>11.878365536902121</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -705,7 +704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -716,7 +715,7 @@
         <v>10.608203677510607</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -727,7 +726,7 @@
         <v>13.130252100840337</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -738,7 +737,7 @@
         <v>11.875439831104856</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -749,7 +748,7 @@
         <v>11.904761904761903</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -760,7 +759,7 @@
         <v>16.660970608339031</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -771,7 +770,7 @@
         <v>15.679442508710801</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -782,7 +781,7 @@
         <v>18.610421836228287</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -793,7 +792,7 @@
         <v>21.699819168173601</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -804,7 +803,7 @@
         <v>24.289312702410939</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -815,7 +814,7 @@
         <v>27.974636329727712</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -826,7 +825,7 @@
         <v>20.447110141766633</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -837,7 +836,7 @@
         <v>32.467532467532465</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -848,7 +847,7 @@
         <v>20.089285714285715</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -859,7 +858,7 @@
         <v>27.262813522355511</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -870,7 +869,7 @@
         <v>29.24494859978731</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -881,7 +880,7 @@
         <v>33.150636492220649</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -892,7 +891,7 @@
         <v>20.395213923132705</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -903,7 +902,7 @@
         <v>28.698979591836736</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -914,7 +913,7 @@
         <v>31.83831672203765</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -925,7 +924,7 @@
         <v>35.991140642303428</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -936,7 +935,7 @@
         <v>35.622944830105958</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -948,7 +947,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -959,7 +958,7 @@
         <v>11.4795918367347</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -970,7 +969,7 @@
         <v>12.846865364850975</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -981,7 +980,7 @@
         <v>7.7639751552795033</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -992,7 +991,7 @@
         <v>18.382352941176471</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1002,7 @@
         <v>3.7904312668463613</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -1014,7 +1013,7 @@
         <v>14.097744360902256</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>23.987206823027716</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>13.098148794970312</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>16.071428571428573</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -1058,7 +1057,7 @@
         <v>26.260504201680675</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1068,7 @@
         <v>24.645451400899343</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -1080,7 +1079,7 @@
         <v>19.363166953528399</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>22.266852951449518</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>24.645451400899343</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>30.199579831932787</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>22.742587601078167</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>28.536838464199239</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -1146,7 +1145,7 @@
         <v>20.31144211238998</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>34.165451895043731</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>37.765759045132405</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -1179,7 +1178,7 @@
         <v>42.40482472672447</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1190,7 @@
       </c>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -1202,7 +1201,7 @@
         <v>13.260254596888261</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -1213,7 +1212,7 @@
         <v>11.934229137199434</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -1224,7 +1223,7 @@
         <v>3.9879475363346333</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>14.550264550264542</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1245,7 @@
         <v>7.8206465067778934</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -1257,7 +1256,7 @@
         <v>11.562178828365877</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1267,7 @@
         <v>58.813501534265257</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -1279,7 +1278,7 @@
         <v>39.960039960039964</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1289,7 @@
         <v>49.603174603174594</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1300,7 @@
         <v>21.060021060021057</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>41.011619958988383</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1322,7 @@
         <v>33.401849948612536</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>8</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>14.622474299893645</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>8</v>
       </c>
@@ -1345,7 +1344,7 @@
         <v>17.027593433461405</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>24.474256707759249</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>22.598369372562932</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -1378,7 +1377,7 @@
         <v>24.412296564195298</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>30.88077336197637</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1399,7 @@
         <v>50.954829232464192</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>8</v>
       </c>
@@ -1411,7 +1410,7 @@
         <v>28.77237851662403</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>8</v>
       </c>
@@ -1422,7 +1421,7 @@
         <v>44.316996871741402</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>0</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>9</v>
       </c>
@@ -1444,7 +1443,7 @@
         <v>13.037294563843234</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1454,7 @@
         <v>22.530040053404541</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -1466,7 +1465,7 @@
         <v>22.419760855884203</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -1477,7 +1476,7 @@
         <v>22.568894520114032</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>22.747952684258426</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>9</v>
       </c>
@@ -1499,7 +1498,7 @@
         <v>18.558231606730455</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>27.626521460602181</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>9</v>
       </c>
@@ -1521,7 +1520,7 @@
         <v>23.238747553816047</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1531,7 @@
         <v>32.798833819241977</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -1543,7 +1542,7 @@
         <v>31.441470493389232</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -1554,7 +1553,7 @@
         <v>32.650757820058047</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>9</v>
       </c>
@@ -1565,7 +1564,7 @@
         <v>40.828109534806991</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>9</v>
       </c>
@@ -1576,7 +1575,7 @@
         <v>38.265306122448983</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1586,7 @@
         <v>33.17496723460026</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -1598,7 +1597,7 @@
         <v>37.462537462537462</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1608,7 @@
         <v>27.093596059113302</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>34.275558564658091</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>40.454396861719509</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -1642,7 +1641,7 @@
         <v>52.497613744829785</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -1653,7 +1652,7 @@
         <v>40.087463556851311</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>9</v>
       </c>
@@ -1668,16 +1667,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D8936B-6596-4A00-B6F7-6450FC096413}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>